<commit_message>
Contour Definition partial convex hull
</commit_message>
<xml_diff>
--- a/Data/Documents/Thesis Reference/Pavlidis' Algorithm (Orientational Pattern).xlsx
+++ b/Data/Documents/Thesis Reference/Pavlidis' Algorithm (Orientational Pattern).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>SWITCH</t>
   </si>
@@ -64,13 +64,37 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>R-1 C-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R-1 </t>
+  </si>
+  <si>
+    <t>dementor</t>
+  </si>
+  <si>
+    <t>R-1 C+1</t>
+  </si>
+  <si>
+    <t>S = dementor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +140,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,8 +175,14 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -235,6 +272,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -244,18 +322,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
@@ -265,6 +340,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -566,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -578,211 +677,580 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="5"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="K5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="10"/>
+      <c r="B13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="10"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="10"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="18"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="14">
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B31:I37"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="G1:I1"/>

</xml_diff>